<commit_message>
add pos and role
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mid-term" sheetId="1" r:id="rId1"/>
+    <sheet name="Binary Classification" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Full</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t>Verb (Similarity)</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Seq2Seq</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Text + POS</t>
+  </si>
+  <si>
+    <t>Text + Role</t>
+  </si>
+  <si>
+    <t>Text + POS + Role</t>
+  </si>
+  <si>
+    <t>Alignment</t>
   </si>
 </sst>
 </file>
@@ -147,7 +172,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -185,12 +210,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -209,6 +243,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -227,6 +264,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -265,7 +305,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$C$2</c:f>
+              <c:f>'Mid-term'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -277,7 +317,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$3:$B$7</c:f>
+              <c:f>'Mid-term'!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -300,7 +340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$C$3:$C$7</c:f>
+              <c:f>'Mid-term'!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -328,7 +368,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$D$2</c:f>
+              <c:f>'Mid-term'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -340,7 +380,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$3:$B$7</c:f>
+              <c:f>'Mid-term'!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -363,7 +403,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$D$3:$D$7</c:f>
+              <c:f>'Mid-term'!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -391,7 +431,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$E$2</c:f>
+              <c:f>'Mid-term'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -403,7 +443,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$3:$B$7</c:f>
+              <c:f>'Mid-term'!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -426,7 +466,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$E$3:$E$7</c:f>
+              <c:f>'Mid-term'!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -458,11 +498,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095937680"/>
-        <c:axId val="-2068696336"/>
+        <c:axId val="-2130099136"/>
+        <c:axId val="2078618592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095937680"/>
+        <c:axId val="-2130099136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +525,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2068696336"/>
+        <c:crossAx val="2078618592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2068696336"/>
+        <c:axId val="2078618592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.6"/>
@@ -518,7 +558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095937680"/>
+        <c:crossAx val="-2130099136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -635,7 +675,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$C$14</c:f>
+              <c:f>'Mid-term'!$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -656,7 +696,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$15:$B$20</c:f>
+              <c:f>'Mid-term'!$B$15:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -682,7 +722,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$C$15:$C$20</c:f>
+              <c:f>'Mid-term'!$C$15:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -713,7 +753,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$D$14</c:f>
+              <c:f>'Mid-term'!$D$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -734,7 +774,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$15:$B$20</c:f>
+              <c:f>'Mid-term'!$B$15:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -760,7 +800,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$D$15:$D$20</c:f>
+              <c:f>'Mid-term'!$D$15:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -791,7 +831,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$E$14</c:f>
+              <c:f>'Mid-term'!$E$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -812,7 +852,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$15:$B$20</c:f>
+              <c:f>'Mid-term'!$B$15:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -838,7 +878,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$E$15:$E$20</c:f>
+              <c:f>'Mid-term'!$E$15:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -874,11 +914,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="-2067298160"/>
-        <c:axId val="-2094896832"/>
+        <c:axId val="-2126957712"/>
+        <c:axId val="-2126954688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2067298160"/>
+        <c:axId val="-2126957712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094896832"/>
+        <c:crossAx val="-2126954688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -929,7 +969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2094896832"/>
+        <c:axId val="-2126954688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1037,7 +1077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067298160"/>
+        <c:crossAx val="-2126957712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -2051,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2279,4 +2319,236 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.996</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(C2+D2)/2</f>
+        <v>0.96849999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E15" si="0">(C3+D3)/2</f>
+        <v>0.96350000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74449999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0.625</v>
+      </c>
+      <c r="D6">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66049999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70700000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>0.876</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.91</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>